<commit_message>
Altered the wording of definitions of done
</commit_message>
<xml_diff>
--- a/Product Backlog/ProductBacklog-1.xlsx
+++ b/Product Backlog/ProductBacklog-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School_Work\Uni\Computer_Science\2022\Semester_2\Process_and_Tools\Assignment1\Milestone1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40AFA7B-21FD-4FD7-9D9A-FBCC769CE40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EE068B-7142-4BD1-85F6-7B418E740501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-10215" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -118,24 +118,6 @@
     <t xml:space="preserve">Doctor landing page </t>
   </si>
   <si>
-    <t>Doctor is presented the landing page when first loading into the website after signing in.</t>
-  </si>
-  <si>
-    <t>Patient is presented the landing page when first loading into the website after signing in.</t>
-  </si>
-  <si>
-    <t>Super Administrator is presented the landing page when first loading into the website after signing in.</t>
-  </si>
-  <si>
-    <t>Navigation bar succesfully displays and provides interaction between pages that the patient can access.</t>
-  </si>
-  <si>
-    <t>Navigation bar succesfully displays and provides interaction between pages that the doctor can access.</t>
-  </si>
-  <si>
-    <t>Navigation bar succesfully displays and provides interaction between pages that the super administrator can access.</t>
-  </si>
-  <si>
     <t>Will welcome the patient to the system as well as provide links to frequently accessed pages that the patient has access to</t>
   </si>
   <si>
@@ -152,6 +134,24 @@
   </si>
   <si>
     <t>Will include pages; create user, view all users, edit users. In addition the super administrator can view all pages the doctor and patient users can view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I sign in, when I load into the website then the first page, I am present with is a landing page tailored to me as a patient. </t>
+  </si>
+  <si>
+    <t>Given that I sign in, when I load into the website then the first page, I am present with is a landing page tailored to me as a doctor.</t>
+  </si>
+  <si>
+    <t>Given that I sign in, when I load into the website then the first page, I am present with is a landing page tailored to me as a super administrator.</t>
+  </si>
+  <si>
+    <t>Given that I am a patient, when I need to access my health info, view my calendar or have a chat with my doctor then I can access the appropriate pages for those tasks through the navigation bar.</t>
+  </si>
+  <si>
+    <t>Given that I am a doctor, when I need to edit my availabilities, view my patients, chat with my patients or access patient prescriptions, then I can access the appropriate pages for those tasks through the navigation bar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a super administrator, when I need to view users, view each user type’s point of view on the website whether it be a patient or doctor, edit users or create new users, then I can access the appropriate pages for those tasks through the navigation bar. </t>
   </si>
 </sst>
 </file>
@@ -831,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -904,7 +904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="22" customFormat="1" ht="38.25">
+    <row r="5" spans="1:9" s="22" customFormat="1" ht="51">
       <c r="A5" s="18"/>
       <c r="B5" s="19">
         <v>1</v>
@@ -925,13 +925,13 @@
         <v>20</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="22" customFormat="1" ht="38.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="22" customFormat="1" ht="51">
       <c r="A6" s="18"/>
       <c r="B6" s="20">
         <v>2</v>
@@ -952,13 +952,13 @@
         <v>20</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="22" customFormat="1" ht="38.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="22" customFormat="1" ht="51">
       <c r="A7" s="18"/>
       <c r="B7" s="20">
         <v>3</v>
@@ -979,13 +979,13 @@
         <v>20</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="22" customFormat="1" ht="38.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="22" customFormat="1" ht="76.5">
       <c r="A8" s="18"/>
       <c r="B8" s="20">
         <v>4</v>
@@ -1006,13 +1006,13 @@
         <v>20</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="22" customFormat="1" ht="38.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="22" customFormat="1" ht="89.25">
       <c r="A9" s="18"/>
       <c r="B9" s="20">
         <v>5</v>
@@ -1033,13 +1033,13 @@
         <v>20</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="22" customFormat="1" ht="51">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="22" customFormat="1" ht="102">
       <c r="A10" s="18"/>
       <c r="B10" s="19">
         <v>6</v>
@@ -1060,10 +1060,10 @@
         <v>20</v>
       </c>
       <c r="H10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="28" t="s">
         <v>30</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="22" customFormat="1">

</xml_diff>

<commit_message>
Add my contribution videos and product backlogs
</commit_message>
<xml_diff>
--- a/Product Backlog/ProductBacklog-1.xlsx
+++ b/Product Backlog/ProductBacklog-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\death\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\repo_my\COSC2299_Group8_Major_Assessment\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3050C983-C832-4DB3-8836-B0228A39DC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E116B7-6722-450C-BCF4-F4BEF6689897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,14 @@
     <definedName name="lstYears">OFFSET('Product Backlog'!$C$4:$I$4,0,1,1,COUNTA('Product Backlog'!$C$4:$I$4)-1)</definedName>
     <definedName name="SelectedYear">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -213,6 +215,75 @@
   </si>
   <si>
     <t>This will update patients details in the  database.</t>
+  </si>
+  <si>
+    <t>Main Page</t>
+  </si>
+  <si>
+    <t>All users</t>
+  </si>
+  <si>
+    <t>Doctor Sign Up Page</t>
+  </si>
+  <si>
+    <t>Patient Sign Up Page</t>
+  </si>
+  <si>
+    <t>Admin Sign Up Page</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Given that I am a doctor, when I get a job in Neighborhood Doctors and am ready to make an account, then I am able to sign up with my email, password and doctor role or another services such as Google etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a user whoever is doctor, patient or admin, when I want to learn more about Neighborhood Doctors and create an account or log in my account, then I am able to log in to the system or choose whether I should create an account. </t>
+  </si>
+  <si>
+    <t>Given that I am a patient, when I feel sick and want to make an account in Neighborhood Doctors, then I am able to sign up with my email, password and patient role or another services such as Google etc.</t>
+  </si>
+  <si>
+    <t>No need to make a checking function for the patient role.</t>
+  </si>
+  <si>
+    <t>Need to add the introduction about Neighborhood Doctors.</t>
+  </si>
+  <si>
+    <t>Will have a checking function whether this user is a doctor.</t>
+  </si>
+  <si>
+    <t>Given that I am an admin, when I get a job as a developer in Neighborhood Doctors and am ready to make an account, then I am able to sign up with my email, password and admin role or another services such as Google etc.</t>
+  </si>
+  <si>
+    <t>Will have a checking function whether this user is a admin.</t>
+  </si>
+  <si>
+    <t>Doctor Log In Page</t>
+  </si>
+  <si>
+    <t>Patient Log In Page</t>
+  </si>
+  <si>
+    <t>Admin Log In Page</t>
+  </si>
+  <si>
+    <t>Given that I am a doctor, when I prepare for working in Neighborhood Doctors, then I am able to log in with my email and password or another services such as Google etc.</t>
+  </si>
+  <si>
+    <t>Given that I am a patient, when I want to log in to Neighborhood Doctors,then I am able to log in with my email and password or another services such as Google etc.</t>
+  </si>
+  <si>
+    <t>Given that I am an admin, when I am about to do the maintance job in Neighborhood Doctors, then I am able to log in with my email and password or another services such as Google etc.</t>
+  </si>
+  <si>
+    <t>Access the doctor information from the database.</t>
+  </si>
+  <si>
+    <t>Access the patient information from the database.</t>
+  </si>
+  <si>
+    <t>Access the admin information from the database.</t>
   </si>
 </sst>
 </file>
@@ -220,10 +291,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color theme="1" tint="0.34998626667073579"/>
@@ -422,7 +493,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3">
+    <xf numFmtId="5" fontId="5" fillId="0" borderId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0">
@@ -496,7 +567,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -505,7 +576,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -517,7 +588,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -892,29 +963,29 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="30" customWidth="1"/>
     <col min="5" max="5" width="11" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="33" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="31.85546875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="33" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="30" customWidth="1"/>
+    <col min="8" max="8" width="31.88671875" style="30" customWidth="1"/>
     <col min="9" max="9" width="68" style="30" customWidth="1"/>
     <col min="10" max="10" width="2" style="30" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="30"/>
+    <col min="11" max="16384" width="8.88671875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" customFormat="1" ht="8.25" customHeight="1">
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" customFormat="1" ht="38.25" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
@@ -927,7 +998,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" customFormat="1" ht="6" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="14"/>
@@ -938,7 +1009,7 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" customFormat="1" ht="25.5" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="15" t="s">
         <v>1</v>
@@ -965,7 +1036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="22" customFormat="1" ht="55.2">
       <c r="A5" s="18"/>
       <c r="B5" s="19">
         <v>1</v>
@@ -992,7 +1063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="22" customFormat="1" ht="55.2">
       <c r="A6" s="18"/>
       <c r="B6" s="20">
         <v>2</v>
@@ -1019,7 +1090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="22" customFormat="1" ht="55.2">
       <c r="A7" s="18"/>
       <c r="B7" s="20">
         <v>3</v>
@@ -1046,7 +1117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="22" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="22" customFormat="1" ht="82.8">
       <c r="A8" s="18"/>
       <c r="B8" s="20">
         <v>4</v>
@@ -1073,7 +1144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="22" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="22" customFormat="1" ht="82.8">
       <c r="A9" s="18"/>
       <c r="B9" s="20">
         <v>5</v>
@@ -1100,7 +1171,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="22" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="22" customFormat="1" ht="110.4">
       <c r="A10" s="18"/>
       <c r="B10" s="19">
         <v>6</v>
@@ -1127,7 +1198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="22" customFormat="1" ht="55.2">
       <c r="A11" s="18"/>
       <c r="B11" s="20">
         <v>7</v>
@@ -1154,7 +1225,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="22" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="22" customFormat="1" ht="69">
       <c r="A12" s="18"/>
       <c r="B12" s="20">
         <v>8</v>
@@ -1181,7 +1252,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="22" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="22" customFormat="1" ht="69">
       <c r="A13" s="18"/>
       <c r="B13" s="20">
         <v>9</v>
@@ -1208,7 +1279,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="22" customFormat="1" ht="55.2">
       <c r="A14" s="18"/>
       <c r="B14" s="20">
         <v>10</v>
@@ -1235,7 +1306,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="22" customFormat="1" ht="55.2">
       <c r="A15" s="18"/>
       <c r="B15" s="19">
         <v>11</v>
@@ -1262,7 +1333,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="22" customFormat="1" ht="55.2">
       <c r="A16" s="18"/>
       <c r="B16" s="20">
         <v>12</v>
@@ -1289,7 +1360,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="22" customFormat="1" ht="55.2">
       <c r="A17" s="18"/>
       <c r="B17" s="20">
         <v>13</v>
@@ -1316,98 +1387,196 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" s="22" customFormat="1" ht="96.6">
       <c r="A18" s="18"/>
       <c r="B18" s="20">
         <v>14</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-    </row>
-    <row r="19" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="27">
+        <v>10</v>
+      </c>
+      <c r="F18" s="27">
+        <v>4</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="22" customFormat="1" ht="82.8">
       <c r="A19" s="18"/>
       <c r="B19" s="20">
         <v>15</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="27">
+        <v>10</v>
+      </c>
+      <c r="F19" s="27">
+        <v>5</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="82.8">
       <c r="A20" s="10"/>
       <c r="B20" s="19">
         <v>16</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C20" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="27">
+        <v>10</v>
+      </c>
+      <c r="F20" s="27">
+        <v>5</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="82.8">
       <c r="A21" s="10"/>
       <c r="B21" s="20">
         <v>17</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C21" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="27">
+        <v>10</v>
+      </c>
+      <c r="F21" s="27">
+        <v>5</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="69">
       <c r="A22" s="10"/>
       <c r="B22" s="20">
         <v>18</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C22" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="27">
+        <v>10</v>
+      </c>
+      <c r="F22" s="27">
+        <v>5</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="69">
       <c r="A23" s="10"/>
       <c r="B23" s="20">
         <v>19</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C23" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="27">
+        <v>10</v>
+      </c>
+      <c r="F23" s="27">
+        <v>5</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="69">
       <c r="A24" s="10"/>
       <c r="B24" s="20">
         <v>20</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C24" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="27">
+        <v>10</v>
+      </c>
+      <c r="F24" s="27">
+        <v>5</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="10"/>
       <c r="B25" s="19">
         <v>21</v>
@@ -1420,7 +1589,7 @@
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="10"/>
       <c r="B26" s="20">
         <v>22</v>
@@ -1433,7 +1602,7 @@
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="10"/>
       <c r="B27" s="20">
         <v>23</v>
@@ -1446,7 +1615,7 @@
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="10"/>
       <c r="B28" s="20">
         <v>24</v>
@@ -1459,7 +1628,7 @@
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="10"/>
       <c r="B29" s="20">
         <v>25</v>
@@ -1472,7 +1641,7 @@
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="10"/>
       <c r="B30" s="19">
         <v>26</v>
@@ -1485,7 +1654,7 @@
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="10"/>
       <c r="B31" s="20">
         <v>27</v>
@@ -1498,7 +1667,7 @@
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="10"/>
       <c r="B32" s="20">
         <v>28</v>
@@ -1511,7 +1680,7 @@
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="10"/>
       <c r="B33" s="20">
         <v>29</v>
@@ -1524,7 +1693,7 @@
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="10"/>
       <c r="B34" s="20">
         <v>30</v>
@@ -1537,7 +1706,7 @@
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="10"/>
       <c r="B35" s="19">
         <v>31</v>
@@ -1550,7 +1719,7 @@
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="10"/>
       <c r="B36" s="20">
         <v>32</v>
@@ -1563,7 +1732,7 @@
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="10"/>
       <c r="B37" s="20">
         <v>33</v>
@@ -1576,7 +1745,7 @@
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="10"/>
       <c r="B38" s="20">
         <v>34</v>
@@ -1589,7 +1758,7 @@
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="10"/>
       <c r="B39" s="19">
         <v>35</v>
@@ -1602,7 +1771,7 @@
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="10"/>
       <c r="B40" s="20">
         <v>36</v>
@@ -1615,7 +1784,7 @@
       <c r="H40" s="28"/>
       <c r="I40" s="28"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="10"/>
       <c r="B41" s="20">
         <v>37</v>
@@ -1628,7 +1797,7 @@
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="10"/>
       <c r="B42" s="20">
         <v>38</v>
@@ -1641,7 +1810,7 @@
       <c r="H42" s="28"/>
       <c r="I42" s="28"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="10"/>
       <c r="B43" s="20">
         <v>39</v>
@@ -1654,7 +1823,7 @@
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="10"/>
       <c r="B44" s="19">
         <v>40</v>
@@ -1667,7 +1836,7 @@
       <c r="H44" s="28"/>
       <c r="I44" s="28"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="10"/>
       <c r="B45" s="21"/>
     </row>
@@ -1709,22 +1878,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="34.5" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="6" customFormat="1">
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="19.5" customHeight="1">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -1737,7 +1906,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="19.5" customHeight="1">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -1750,8 +1919,8 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="19.5" customHeight="1"/>
+    <row r="6" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -1776,7 +1945,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18" thickBot="1">
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1802,7 +1971,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1">
       <c r="A8" t="e">
         <f>MATCH(B8,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -1836,7 +2005,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="19.5" customHeight="1">
       <c r="A9" t="e">
         <f>MATCH(B9,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -1870,7 +2039,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="19.5" customHeight="1">
       <c r="A10" t="e">
         <f>MATCH(B10,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -1904,7 +2073,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="19.5" customHeight="1">
       <c r="A11" t="e">
         <f>MATCH(B11,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -1938,7 +2107,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="19.5" customHeight="1">
       <c r="A12" t="e">
         <f>MATCH(B12,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -1972,8 +2141,8 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="13.8" thickBot="1"/>
+    <row r="14" spans="1:8" ht="18" thickBot="1">
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1984,7 +2153,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="19.5" customHeight="1">
       <c r="A15">
         <f>ROWS($B$15:B15)</f>
         <v>1</v>
@@ -2014,7 +2183,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="19.5" customHeight="1">
       <c r="A16">
         <f>ROWS($B$15:B16)</f>
         <v>2</v>
@@ -2044,7 +2213,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="19.5" customHeight="1">
       <c r="A17">
         <f>ROWS($B$15:B17)</f>
         <v>3</v>
@@ -2074,7 +2243,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="19.5" customHeight="1">
       <c r="A18">
         <f>ROWS($B$15:B18)</f>
         <v>4</v>
@@ -2104,7 +2273,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="19.5" customHeight="1">
       <c r="A19">
         <f>ROWS($B$15:B19)</f>
         <v>5</v>
@@ -2134,7 +2303,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="19.5" customHeight="1">
       <c r="A20">
         <f>ROWS($B$15:B20)</f>
         <v>6</v>
@@ -2164,7 +2333,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="19.5" customHeight="1">
       <c r="A21">
         <f>ROWS($B$15:B21)</f>
         <v>7</v>
@@ -2194,7 +2363,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="19.5" customHeight="1">
       <c r="A22">
         <f>ROWS($B$15:B22)</f>
         <v>8</v>
@@ -2224,7 +2393,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="19.5" customHeight="1">
       <c r="A23">
         <f>ROWS($B$15:B23)</f>
         <v>9</v>
@@ -2254,7 +2423,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="19.5" customHeight="1">
       <c r="A24">
         <f>ROWS($B$15:B24)</f>
         <v>10</v>
@@ -2284,7 +2453,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="19.5" customHeight="1">
       <c r="A25">
         <f>ROWS($B$15:B25)</f>
         <v>11</v>
@@ -2314,7 +2483,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="19.5" customHeight="1">
       <c r="A26">
         <f>ROWS($B$15:B26)</f>
         <v>12</v>
@@ -2344,7 +2513,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="19.5" customHeight="1">
       <c r="A27">
         <f>ROWS($B$15:B27)</f>
         <v>13</v>
@@ -2374,217 +2543,217 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="19.5" customHeight="1">
       <c r="A28">
         <f>ROWS($B$15:B28)</f>
         <v>14</v>
       </c>
       <c r="B28" t="str">
         <f>IF('Product Backlog'!C18=0,"",'Product Backlog'!C18)</f>
-        <v/>
+        <v>Main Page</v>
       </c>
       <c r="C28" t="e">
-        <f>IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,C$6),NA()))</f>
+        <f ca="1">IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D28" t="e">
-        <f>IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,D$6),NA()))</f>
+        <f ca="1">IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E28" t="e">
-        <f>IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,E$6),NA()))</f>
+        <f ca="1">IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F28" t="e">
-        <f>IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,F$6),NA()))</f>
+        <f ca="1">IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G28" t="e">
-        <f>IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,G$6),NA()))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <f ca="1">IF(B28="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A28,G$6),NA()))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="19.5" customHeight="1">
       <c r="A29">
         <f>ROWS($B$15:B29)</f>
         <v>15</v>
       </c>
       <c r="B29" t="str">
         <f>IF('Product Backlog'!C19=0,"",'Product Backlog'!C19)</f>
-        <v/>
+        <v>Doctor Sign Up Page</v>
       </c>
       <c r="C29" t="e">
-        <f>IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,C$6),NA()))</f>
+        <f ca="1">IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D29" t="e">
-        <f>IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,D$6),NA()))</f>
+        <f ca="1">IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E29" t="e">
-        <f>IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,E$6),NA()))</f>
+        <f ca="1">IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F29" t="e">
-        <f>IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,F$6),NA()))</f>
+        <f ca="1">IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G29" t="e">
-        <f>IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,G$6),NA()))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <f ca="1">IF(B29="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A29,G$6),NA()))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="19.5" customHeight="1">
       <c r="A30">
         <f>ROWS($B$15:B30)</f>
         <v>16</v>
       </c>
       <c r="B30" t="str">
         <f>IF('Product Backlog'!C20=0,"",'Product Backlog'!C20)</f>
-        <v/>
+        <v>Patient Sign Up Page</v>
       </c>
       <c r="C30" t="e">
-        <f>IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,C$6),NA()))</f>
+        <f ca="1">IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D30" t="e">
-        <f>IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,D$6),NA()))</f>
+        <f ca="1">IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E30" t="e">
-        <f>IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,E$6),NA()))</f>
+        <f ca="1">IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F30" t="e">
-        <f>IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,F$6),NA()))</f>
+        <f ca="1">IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G30" t="e">
-        <f>IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,G$6),NA()))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <f ca="1">IF(B30="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A30,G$6),NA()))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="19.5" customHeight="1">
       <c r="A31">
         <f>ROWS($B$15:B31)</f>
         <v>17</v>
       </c>
       <c r="B31" t="str">
         <f>IF('Product Backlog'!C21=0,"",'Product Backlog'!C21)</f>
-        <v/>
+        <v>Admin Sign Up Page</v>
       </c>
       <c r="C31" t="e">
-        <f>IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,C$6),NA()))</f>
+        <f ca="1">IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D31" t="e">
-        <f>IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,D$6),NA()))</f>
+        <f ca="1">IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E31" t="e">
-        <f>IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,E$6),NA()))</f>
+        <f ca="1">IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F31" t="e">
-        <f>IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,F$6),NA()))</f>
+        <f ca="1">IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G31" t="e">
-        <f>IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,G$6),NA()))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <f ca="1">IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,G$6),NA()))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="19.5" customHeight="1">
       <c r="A32">
         <f>ROWS($B$15:B32)</f>
         <v>18</v>
       </c>
       <c r="B32" t="str">
         <f>IF('Product Backlog'!C22=0,"",'Product Backlog'!C22)</f>
-        <v/>
+        <v>Doctor Log In Page</v>
       </c>
       <c r="C32" t="e">
-        <f>IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,C$6),NA()))</f>
+        <f ca="1">IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D32" t="e">
-        <f>IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,D$6),NA()))</f>
+        <f ca="1">IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E32" t="e">
-        <f>IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,E$6),NA()))</f>
+        <f ca="1">IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F32" t="e">
-        <f>IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,F$6),NA()))</f>
+        <f ca="1">IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G32" t="e">
-        <f>IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,G$6),NA()))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <f ca="1">IF(B32="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A32,G$6),NA()))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="19.5" customHeight="1">
       <c r="A33">
         <f>ROWS($B$15:B33)</f>
         <v>19</v>
       </c>
       <c r="B33" t="str">
         <f>IF('Product Backlog'!C23=0,"",'Product Backlog'!C23)</f>
-        <v/>
+        <v>Patient Log In Page</v>
       </c>
       <c r="C33" t="e">
-        <f>IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,C$6),NA()))</f>
+        <f ca="1">IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D33" t="e">
-        <f>IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,D$6),NA()))</f>
+        <f ca="1">IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E33" t="e">
-        <f>IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,E$6),NA()))</f>
+        <f ca="1">IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F33" t="e">
-        <f>IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,F$6),NA()))</f>
+        <f ca="1">IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G33" t="e">
-        <f>IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,G$6),NA()))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <f ca="1">IF(B33="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A33,G$6),NA()))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="19.5" customHeight="1">
       <c r="A34">
         <f>ROWS($B$15:B34)</f>
         <v>20</v>
       </c>
       <c r="B34" t="str">
         <f>IF('Product Backlog'!C24=0,"",'Product Backlog'!C24)</f>
-        <v/>
+        <v>Admin Log In Page</v>
       </c>
       <c r="C34" t="e">
-        <f>IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,C$6),NA()))</f>
+        <f ca="1">IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D34" t="e">
-        <f>IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,D$6),NA()))</f>
+        <f ca="1">IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E34" t="e">
-        <f>IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,E$6),NA()))</f>
+        <f ca="1">IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F34" t="e">
-        <f>IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,F$6),NA()))</f>
+        <f ca="1">IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G34" t="e">
-        <f>IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,G$6),NA()))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <f ca="1">IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,G$6),NA()))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="19.5" customHeight="1">
       <c r="A35">
         <f>ROWS($B$15:B35)</f>
         <v>21</v>
@@ -2614,7 +2783,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="19.5" customHeight="1">
       <c r="A36">
         <f>ROWS($B$15:B36)</f>
         <v>22</v>
@@ -2644,7 +2813,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="19.5" customHeight="1">
       <c r="A37">
         <f>ROWS($B$15:B37)</f>
         <v>23</v>
@@ -2674,7 +2843,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="19.5" customHeight="1">
       <c r="A38">
         <f>ROWS($B$15:B38)</f>
         <v>24</v>
@@ -2704,7 +2873,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="19.5" customHeight="1">
       <c r="A39">
         <f>ROWS($B$15:B39)</f>
         <v>25</v>

</xml_diff>

<commit_message>
ProductBacklog and recorded videos (Marco)
</commit_message>
<xml_diff>
--- a/Product Backlog/ProductBacklog-1.xlsx
+++ b/Product Backlog/ProductBacklog-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\repo_my\COSC2299_Group8_Major_Assessment\Product Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\COSC2299_Group8_Major_Assessment\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E116B7-6722-450C-BCF4-F4BEF6689897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2708692F-766A-4E7A-A7FA-54590AF0C73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -229,18 +229,9 @@
     <t>Patient Sign Up Page</t>
   </si>
   <si>
-    <t>Admin Sign Up Page</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>Given that I am a doctor, when I get a job in Neighborhood Doctors and am ready to make an account, then I am able to sign up with my email, password and doctor role or another services such as Google etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given that I am a user whoever is doctor, patient or admin, when I want to learn more about Neighborhood Doctors and create an account or log in my account, then I am able to log in to the system or choose whether I should create an account. </t>
-  </si>
-  <si>
     <t>Given that I am a patient, when I feel sick and want to make an account in Neighborhood Doctors, then I am able to sign up with my email, password and patient role or another services such as Google etc.</t>
   </si>
   <si>
@@ -265,9 +256,6 @@
     <t>Patient Log In Page</t>
   </si>
   <si>
-    <t>Admin Log In Page</t>
-  </si>
-  <si>
     <t>Given that I am a doctor, when I prepare for working in Neighborhood Doctors, then I am able to log in with my email and password or another services such as Google etc.</t>
   </si>
   <si>
@@ -284,6 +272,45 @@
   </si>
   <si>
     <t>Access the admin information from the database.</t>
+  </si>
+  <si>
+    <t>Super Administrator View Page</t>
+  </si>
+  <si>
+    <t>Super Administrator Edit User Page</t>
+  </si>
+  <si>
+    <t>Super Administrator Create User Page</t>
+  </si>
+  <si>
+    <t>Super Administrator</t>
+  </si>
+  <si>
+    <t>Super Administrator Sign Up Page</t>
+  </si>
+  <si>
+    <t>Super Administrator Log In Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a user whoever is doctor, patient or super admin, when I want to learn more about Neighborhood Doctors and create an account or log in my account, then I am able to log in to the system or choose whether I should create an account. </t>
+  </si>
+  <si>
+    <t>Given that I am an admin, when I am going to create a new user, then I am able to add a new user to the system.</t>
+  </si>
+  <si>
+    <t>Given that I am an admin, when I am going to edit user details, then I am able to edit any user details and store it in the system.</t>
+  </si>
+  <si>
+    <t>Given that I am an admin, when I am going to view user details, then I am able to view any user in the system using their unique ID.</t>
+  </si>
+  <si>
+    <t>Access and add new information to the database.</t>
+  </si>
+  <si>
+    <t>Access user information from the database.</t>
+  </si>
+  <si>
+    <t>Access and edit user information from the database.</t>
   </si>
 </sst>
 </file>
@@ -291,8 +318,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -493,7 +520,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="5" fontId="5" fillId="0" borderId="3">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0">
@@ -501,7 +528,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -516,10 +543,7 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyAlignment="1">
@@ -564,47 +588,44 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Key Metric Header" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Key Metric Percentage" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Key Metric Value" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="一般" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="標題" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="標題 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="標題 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="標題 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -963,882 +984,924 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="51.33203125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="11" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="33" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="30" customWidth="1"/>
-    <col min="8" max="8" width="31.88671875" style="30" customWidth="1"/>
-    <col min="9" max="9" width="68" style="30" customWidth="1"/>
-    <col min="10" max="10" width="2" style="30" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="30"/>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="11" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="29" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" style="29" customWidth="1"/>
+    <col min="9" max="9" width="68" style="29" customWidth="1"/>
+    <col min="10" max="10" width="2" style="29" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="8.25" customHeight="1">
-      <c r="B1" s="9"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" customFormat="1" ht="6" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="22" customFormat="1" ht="55.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19">
+    <row r="5" spans="1:9" s="21" customFormat="1" ht="51">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18">
         <v>1</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>8</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>4</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="22" customFormat="1" ht="55.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="20">
+    <row r="6" spans="1:9" s="21" customFormat="1" ht="51">
+      <c r="A6" s="17"/>
+      <c r="B6" s="19">
         <v>2</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <v>8</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="26">
         <v>4</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="22" customFormat="1" ht="55.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="20">
+    <row r="7" spans="1:9" s="21" customFormat="1" ht="51">
+      <c r="A7" s="17"/>
+      <c r="B7" s="19">
         <v>3</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>8</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="26">
         <v>5</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="22" customFormat="1" ht="82.8">
-      <c r="A8" s="18"/>
-      <c r="B8" s="20">
+    <row r="8" spans="1:9" s="21" customFormat="1" ht="76.5">
+      <c r="A8" s="17"/>
+      <c r="B8" s="19">
         <v>4</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <v>10</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="26">
         <v>6</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="22" customFormat="1" ht="82.8">
-      <c r="A9" s="18"/>
-      <c r="B9" s="20">
+    <row r="9" spans="1:9" s="21" customFormat="1" ht="89.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="19">
         <v>5</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <v>10</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="26">
         <v>6</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="22" customFormat="1" ht="110.4">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19">
+    <row r="10" spans="1:9" s="21" customFormat="1" ht="102">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18">
         <v>6</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="26">
         <v>10</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="26">
         <v>7</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="22" customFormat="1" ht="55.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="20">
+    <row r="11" spans="1:9" s="21" customFormat="1" ht="51">
+      <c r="A11" s="17"/>
+      <c r="B11" s="19">
         <v>7</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="28">
         <v>8</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="26">
         <v>8</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="22" customFormat="1" ht="69">
-      <c r="A12" s="18"/>
-      <c r="B12" s="20">
+    <row r="12" spans="1:9" s="21" customFormat="1" ht="63.75">
+      <c r="A12" s="17"/>
+      <c r="B12" s="19">
         <v>8</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="26">
         <v>10</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="26">
         <v>5</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="22" customFormat="1" ht="69">
-      <c r="A13" s="18"/>
-      <c r="B13" s="20">
+    <row r="13" spans="1:9" s="21" customFormat="1" ht="63.75">
+      <c r="A13" s="17"/>
+      <c r="B13" s="19">
         <v>9</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="26">
         <v>10</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="26">
         <v>7</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="H13" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I13" s="27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="22" customFormat="1" ht="55.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="20">
+    <row r="14" spans="1:9" s="21" customFormat="1" ht="51">
+      <c r="A14" s="17"/>
+      <c r="B14" s="19">
         <v>10</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="26">
         <v>5</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="26">
         <v>5</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="22" customFormat="1" ht="55.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19">
+    <row r="15" spans="1:9" s="21" customFormat="1" ht="51">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18">
         <v>11</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="26">
         <v>8</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="26">
         <v>5</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="22" customFormat="1" ht="55.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="20">
+    <row r="16" spans="1:9" s="21" customFormat="1" ht="51">
+      <c r="A16" s="17"/>
+      <c r="B16" s="19">
         <v>12</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="26">
         <v>8</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="26">
         <v>4</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="22" customFormat="1" ht="55.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="20">
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="51">
+      <c r="A17" s="17"/>
+      <c r="B17" s="19">
         <v>13</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="26">
         <v>4</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="26">
         <v>5</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="H17" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="22" customFormat="1" ht="96.6">
-      <c r="A18" s="18"/>
-      <c r="B18" s="20">
+    <row r="18" spans="1:9" s="21" customFormat="1" ht="102">
+      <c r="A18" s="17"/>
+      <c r="B18" s="19">
         <v>14</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="26">
         <v>10</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="26">
         <v>4</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="28" t="s">
+      <c r="H18" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="I18" s="28" t="s">
+    </row>
+    <row r="19" spans="1:9" s="21" customFormat="1" ht="76.5">
+      <c r="A19" s="17"/>
+      <c r="B19" s="19">
+        <v>15</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="26">
+        <v>10</v>
+      </c>
+      <c r="F19" s="26">
+        <v>5</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="76.5">
+      <c r="A20" s="9"/>
+      <c r="B20" s="18">
+        <v>16</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="26">
+        <v>10</v>
+      </c>
+      <c r="F20" s="26">
+        <v>5</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="76.5">
+      <c r="A21" s="9"/>
+      <c r="B21" s="19">
+        <v>17</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="26">
+        <v>10</v>
+      </c>
+      <c r="F21" s="26">
+        <v>5</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="27" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="22" customFormat="1" ht="82.8">
-      <c r="A19" s="18"/>
-      <c r="B19" s="20">
-        <v>15</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="26" t="s">
+    <row r="22" spans="1:9" ht="63.75">
+      <c r="A22" s="9"/>
+      <c r="B22" s="19">
+        <v>18</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E22" s="26">
         <v>10</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F22" s="26">
         <v>5</v>
       </c>
-      <c r="G19" s="28" t="s">
+      <c r="G22" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="82.8">
-      <c r="A20" s="10"/>
-      <c r="B20" s="19">
-        <v>16</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="26" t="s">
+      <c r="H22" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="63.75">
+      <c r="A23" s="9"/>
+      <c r="B23" s="19">
+        <v>19</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E23" s="26">
         <v>10</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F23" s="26">
         <v>5</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G23" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="82.8">
-      <c r="A21" s="10"/>
-      <c r="B21" s="20">
-        <v>17</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="27">
+      <c r="H23" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="76.5">
+      <c r="A24" s="9"/>
+      <c r="B24" s="19">
+        <v>20</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="26">
         <v>10</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F24" s="26">
         <v>5</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G24" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="69">
-      <c r="A22" s="10"/>
-      <c r="B22" s="20">
-        <v>18</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="27">
-        <v>10</v>
-      </c>
-      <c r="F22" s="27">
-        <v>5</v>
-      </c>
-      <c r="G22" s="28" t="s">
+      <c r="H24" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="38.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="18">
+        <v>21</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="26">
+        <v>8</v>
+      </c>
+      <c r="F25" s="26">
+        <v>6</v>
+      </c>
+      <c r="G25" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="28" t="s">
+      <c r="H25" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="51">
+      <c r="A26" s="9"/>
+      <c r="B26" s="19">
+        <v>22</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="26">
+        <v>8</v>
+      </c>
+      <c r="F26" s="26">
+        <v>7</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="51">
+      <c r="A27" s="9"/>
+      <c r="B27" s="19">
+        <v>23</v>
+      </c>
+      <c r="C27" s="25" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="69">
-      <c r="A23" s="10"/>
-      <c r="B23" s="20">
-        <v>19</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="27">
-        <v>10</v>
-      </c>
-      <c r="F23" s="27">
-        <v>5</v>
-      </c>
-      <c r="G23" s="28" t="s">
+      <c r="D27" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="26">
+        <v>8</v>
+      </c>
+      <c r="F27" s="26">
+        <v>7</v>
+      </c>
+      <c r="G27" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="I23" s="28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="69">
-      <c r="A24" s="10"/>
-      <c r="B24" s="20">
-        <v>20</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="27">
-        <v>10</v>
-      </c>
-      <c r="F24" s="27">
-        <v>5</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="10"/>
-      <c r="B25" s="19">
-        <v>21</v>
-      </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="10"/>
-      <c r="B26" s="20">
-        <v>22</v>
-      </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="10"/>
-      <c r="B27" s="20">
-        <v>23</v>
-      </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
+      <c r="H27" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="10"/>
-      <c r="B28" s="20">
+      <c r="A28" s="9"/>
+      <c r="B28" s="19">
         <v>24</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="10"/>
-      <c r="B29" s="20">
+      <c r="A29" s="9"/>
+      <c r="B29" s="19">
         <v>25</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="10"/>
-      <c r="B30" s="19">
+      <c r="A30" s="9"/>
+      <c r="B30" s="18">
         <v>26</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="10"/>
-      <c r="B31" s="20">
+      <c r="A31" s="9"/>
+      <c r="B31" s="19">
         <v>27</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="10"/>
-      <c r="B32" s="20">
+      <c r="A32" s="9"/>
+      <c r="B32" s="19">
         <v>28</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="10"/>
-      <c r="B33" s="20">
+      <c r="A33" s="9"/>
+      <c r="B33" s="19">
         <v>29</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="10"/>
-      <c r="B34" s="20">
+      <c r="A34" s="9"/>
+      <c r="B34" s="19">
         <v>30</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="10"/>
-      <c r="B35" s="19">
+      <c r="A35" s="9"/>
+      <c r="B35" s="18">
         <v>31</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="10"/>
-      <c r="B36" s="20">
+      <c r="A36" s="9"/>
+      <c r="B36" s="19">
         <v>32</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="10"/>
-      <c r="B37" s="20">
+      <c r="A37" s="9"/>
+      <c r="B37" s="19">
         <v>33</v>
       </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="10"/>
-      <c r="B38" s="20">
+      <c r="A38" s="9"/>
+      <c r="B38" s="19">
         <v>34</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="10"/>
-      <c r="B39" s="19">
+      <c r="A39" s="9"/>
+      <c r="B39" s="18">
         <v>35</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="10"/>
-      <c r="B40" s="20">
+      <c r="A40" s="9"/>
+      <c r="B40" s="19">
         <v>36</v>
       </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="10"/>
-      <c r="B41" s="20">
+      <c r="A41" s="9"/>
+      <c r="B41" s="19">
         <v>37</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="10"/>
-      <c r="B42" s="20">
+      <c r="A42" s="9"/>
+      <c r="B42" s="19">
         <v>38</v>
       </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="10"/>
-      <c r="B43" s="20">
+      <c r="A43" s="9"/>
+      <c r="B43" s="19">
         <v>39</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="10"/>
-      <c r="B44" s="19">
+      <c r="A44" s="9"/>
+      <c r="B44" s="18">
         <v>40</v>
       </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="10"/>
-      <c r="B45" s="21"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:I6 B7:B10 H7:I10 C8:G10 B11:I44">
@@ -1878,17 +1941,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" ht="34.5" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1">
+    <row r="2" spans="1:8">
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1945,27 +2008,27 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" thickBot="1">
+    <row r="7" spans="1:8" ht="18.75" thickBot="1">
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8" t="e">
+      <c r="C7" s="7" t="e">
         <f>D7-1</f>
         <v>#REF!</v>
       </c>
-      <c r="D7" s="8" t="e">
+      <c r="D7" s="7" t="e">
         <f>E7-1</f>
         <v>#REF!</v>
       </c>
-      <c r="E7" s="8" t="e">
+      <c r="E7" s="7" t="e">
         <f>F7-1</f>
         <v>#REF!</v>
       </c>
-      <c r="F7" s="8" t="e">
+      <c r="F7" s="7" t="e">
         <f>G7-1</f>
         <v>#REF!</v>
       </c>
-      <c r="G7" s="8" t="e">
+      <c r="G7" s="7" t="e">
         <f>C3</f>
         <v>#REF!</v>
       </c>
@@ -2141,8 +2204,8 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.8" thickBot="1"/>
-    <row r="14" spans="1:8" ht="18" thickBot="1">
+    <row r="13" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="14" spans="1:8" ht="18.75" thickBot="1">
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -2640,7 +2703,7 @@
       </c>
       <c r="B31" t="str">
         <f>IF('Product Backlog'!C21=0,"",'Product Backlog'!C21)</f>
-        <v>Admin Sign Up Page</v>
+        <v>Super Administrator Sign Up Page</v>
       </c>
       <c r="C31" t="e">
         <f ca="1">IF(B31="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A31,C$6),NA()))</f>
@@ -2730,7 +2793,7 @@
       </c>
       <c r="B34" t="str">
         <f>IF('Product Backlog'!C24=0,"",'Product Backlog'!C24)</f>
-        <v>Admin Log In Page</v>
+        <v>Super Administrator Log In Page</v>
       </c>
       <c r="C34" t="e">
         <f ca="1">IF(B34="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A34,C$6),NA()))</f>
@@ -2760,26 +2823,26 @@
       </c>
       <c r="B35" t="str">
         <f>IF('Product Backlog'!C25=0,"",'Product Backlog'!C25)</f>
-        <v/>
+        <v>Super Administrator Create User Page</v>
       </c>
       <c r="C35" t="e">
-        <f>IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,C$6),NA()))</f>
+        <f ca="1">IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D35" t="e">
-        <f>IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,D$6),NA()))</f>
+        <f ca="1">IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E35" t="e">
-        <f>IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,E$6),NA()))</f>
+        <f ca="1">IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F35" t="e">
-        <f>IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,F$6),NA()))</f>
+        <f ca="1">IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G35" t="e">
-        <f>IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,G$6),NA()))</f>
+        <f ca="1">IF(B35="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A35,G$6),NA()))</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2790,26 +2853,26 @@
       </c>
       <c r="B36" t="str">
         <f>IF('Product Backlog'!C26=0,"",'Product Backlog'!C26)</f>
-        <v/>
+        <v>Super Administrator View Page</v>
       </c>
       <c r="C36" t="e">
-        <f>IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,C$6),NA()))</f>
+        <f ca="1">IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D36" t="e">
-        <f>IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,D$6),NA()))</f>
+        <f ca="1">IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E36" t="e">
-        <f>IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,E$6),NA()))</f>
+        <f ca="1">IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F36" t="e">
-        <f>IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,F$6),NA()))</f>
+        <f ca="1">IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G36" t="e">
-        <f>IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,G$6),NA()))</f>
+        <f ca="1">IF(B36="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A36,G$6),NA()))</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2820,26 +2883,26 @@
       </c>
       <c r="B37" t="str">
         <f>IF('Product Backlog'!C27=0,"",'Product Backlog'!C27)</f>
-        <v/>
+        <v>Super Administrator Edit User Page</v>
       </c>
       <c r="C37" t="e">
-        <f>IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,C$6),NA()))</f>
+        <f ca="1">IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D37" t="e">
-        <f>IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,D$6),NA()))</f>
+        <f ca="1">IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E37" t="e">
-        <f>IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,E$6),NA()))</f>
+        <f ca="1">IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F37" t="e">
-        <f>IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,F$6),NA()))</f>
+        <f ca="1">IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G37" t="e">
-        <f>IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,G$6),NA()))</f>
+        <f ca="1">IF(B37="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A37,G$6),NA()))</f>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add final final submission folder a
</commit_message>
<xml_diff>
--- a/Product Backlog/ProductBacklog-1.xlsx
+++ b/Product Backlog/ProductBacklog-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\COSC2299_Group8_Major_Assessment\Product Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\repo_my\COSC2299_Group8_Major_Assessment\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2708692F-766A-4E7A-A7FA-54590AF0C73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D55E53-9A52-402B-ACA9-EF26EC98DE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -318,8 +318,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -520,7 +520,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3">
+    <xf numFmtId="5" fontId="5" fillId="0" borderId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0">
@@ -528,7 +528,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -549,83 +549,98 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Key Metric Header" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Key Metric Percentage" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Key Metric Value" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="一般" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="標題" xfId="2" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="標題 1" xfId="3" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="標題 2" xfId="4" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="標題 3" xfId="8" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -980,928 +995,935 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
-    <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B2" sqref="B2:I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" style="29" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="11" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="29" customWidth="1"/>
-    <col min="8" max="8" width="31.85546875" style="29" customWidth="1"/>
-    <col min="9" max="9" width="68" style="29" customWidth="1"/>
-    <col min="10" max="10" width="2" style="29" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="29"/>
+    <col min="1" max="1" width="1.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.5546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" style="22" customWidth="1"/>
+    <col min="8" max="8" width="31.88671875" style="34" customWidth="1"/>
+    <col min="9" max="9" width="62.5546875" style="34" customWidth="1"/>
+    <col min="10" max="10" width="2" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="8.25" customHeight="1">
-      <c r="B1" s="8"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" customFormat="1" ht="6" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:9" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="21" customFormat="1" ht="51">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18">
+    <row r="5" spans="1:9" s="11" customFormat="1" ht="55.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="15">
         <v>1</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="20">
         <v>8</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>4</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="21" customFormat="1" ht="51">
-      <c r="A6" s="17"/>
-      <c r="B6" s="19">
+    <row r="6" spans="1:9" s="11" customFormat="1" ht="55.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="16">
         <v>2</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="21">
         <v>8</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="21">
         <v>4</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" ht="51">
-      <c r="A7" s="17"/>
-      <c r="B7" s="19">
+    <row r="7" spans="1:9" s="11" customFormat="1" ht="55.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="16">
         <v>3</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="21">
         <v>8</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="21">
         <v>5</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="21" customFormat="1" ht="76.5">
-      <c r="A8" s="17"/>
-      <c r="B8" s="19">
+    <row r="8" spans="1:9" s="11" customFormat="1" ht="82.8">
+      <c r="A8" s="10"/>
+      <c r="B8" s="16">
         <v>4</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="21">
         <v>10</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="21">
         <v>6</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="21" customFormat="1" ht="89.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="19">
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="82.8">
+      <c r="A9" s="10"/>
+      <c r="B9" s="16">
         <v>5</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="21">
         <v>10</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="21">
         <v>6</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="21" customFormat="1" ht="102">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18">
+    <row r="10" spans="1:9" s="11" customFormat="1" ht="110.4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="15">
         <v>6</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="21">
         <v>10</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="21">
         <v>7</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="21" customFormat="1" ht="51">
-      <c r="A11" s="17"/>
-      <c r="B11" s="19">
+    <row r="11" spans="1:9" s="11" customFormat="1" ht="55.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="16">
         <v>7</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="24">
         <v>8</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="21">
         <v>8</v>
       </c>
       <c r="G11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="21" customFormat="1" ht="63.75">
-      <c r="A12" s="17"/>
-      <c r="B12" s="19">
+    <row r="12" spans="1:9" s="11" customFormat="1" ht="69">
+      <c r="A12" s="10"/>
+      <c r="B12" s="16">
         <v>8</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="21">
         <v>10</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="21">
         <v>5</v>
       </c>
       <c r="G12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="21" customFormat="1" ht="63.75">
-      <c r="A13" s="17"/>
-      <c r="B13" s="19">
+    <row r="13" spans="1:9" s="11" customFormat="1" ht="69">
+      <c r="A13" s="10"/>
+      <c r="B13" s="16">
         <v>9</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="21">
         <v>10</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="21">
         <v>7</v>
       </c>
       <c r="G13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="21" customFormat="1" ht="51">
-      <c r="A14" s="17"/>
-      <c r="B14" s="19">
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="55.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="16">
         <v>10</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="21">
         <v>5</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="21">
         <v>5</v>
       </c>
       <c r="G14" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I14" s="32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="21" customFormat="1" ht="51">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18">
+    <row r="15" spans="1:9" s="11" customFormat="1" ht="55.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="15">
         <v>11</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="21">
         <v>8</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="21">
         <v>5</v>
       </c>
       <c r="G15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="21" customFormat="1" ht="51">
-      <c r="A16" s="17"/>
-      <c r="B16" s="19">
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="55.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="16">
         <v>12</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="21">
         <v>8</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="21">
         <v>4</v>
       </c>
       <c r="G16" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="32" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="21" customFormat="1" ht="51">
-      <c r="A17" s="17"/>
-      <c r="B17" s="19">
+    <row r="17" spans="1:9" s="11" customFormat="1" ht="55.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="16">
         <v>13</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="21">
         <v>4</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="21">
         <v>5</v>
       </c>
       <c r="G17" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="21" customFormat="1" ht="102">
-      <c r="A18" s="17"/>
-      <c r="B18" s="19">
+    <row r="18" spans="1:9" s="11" customFormat="1" ht="110.4">
+      <c r="A18" s="10"/>
+      <c r="B18" s="16">
         <v>14</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="21">
         <v>10</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="21">
         <v>4</v>
       </c>
       <c r="G18" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="21" customFormat="1" ht="76.5">
-      <c r="A19" s="17"/>
-      <c r="B19" s="19">
+    <row r="19" spans="1:9" s="11" customFormat="1" ht="82.8">
+      <c r="A19" s="10"/>
+      <c r="B19" s="16">
         <v>15</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="21">
         <v>10</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="21">
         <v>5</v>
       </c>
       <c r="G19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="I19" s="27" t="s">
+      <c r="I19" s="32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="76.5">
-      <c r="A20" s="9"/>
-      <c r="B20" s="18">
+    <row r="20" spans="1:9" ht="82.8">
+      <c r="A20" s="8"/>
+      <c r="B20" s="15">
         <v>16</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="21">
         <v>10</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="21">
         <v>5</v>
       </c>
       <c r="G20" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="76.5">
-      <c r="A21" s="9"/>
-      <c r="B21" s="19">
+    <row r="21" spans="1:9" ht="82.8">
+      <c r="A21" s="8"/>
+      <c r="B21" s="16">
         <v>17</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="21">
         <v>10</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="21">
         <v>5</v>
       </c>
       <c r="G21" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="63.75">
-      <c r="A22" s="9"/>
-      <c r="B22" s="19">
+    <row r="22" spans="1:9" ht="69">
+      <c r="A22" s="8"/>
+      <c r="B22" s="16">
         <v>18</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="21">
         <v>10</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="21">
         <v>5</v>
       </c>
       <c r="G22" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="63.75">
-      <c r="A23" s="9"/>
-      <c r="B23" s="19">
+    <row r="23" spans="1:9" ht="69">
+      <c r="A23" s="8"/>
+      <c r="B23" s="16">
         <v>19</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="26">
+      <c r="E23" s="21">
         <v>10</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="21">
         <v>5</v>
       </c>
       <c r="G23" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="H23" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="I23" s="27" t="s">
+      <c r="I23" s="32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="76.5">
-      <c r="A24" s="9"/>
-      <c r="B24" s="19">
+    <row r="24" spans="1:9" ht="69">
+      <c r="A24" s="8"/>
+      <c r="B24" s="16">
         <v>20</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="21">
         <v>10</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="21">
         <v>5</v>
       </c>
       <c r="G24" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I24" s="27" t="s">
+      <c r="I24" s="32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="38.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="18">
+    <row r="25" spans="1:9" ht="41.4">
+      <c r="A25" s="8"/>
+      <c r="B25" s="15">
         <v>21</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="21">
         <v>8</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="21">
         <v>6</v>
       </c>
       <c r="G25" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="I25" s="32" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="51">
-      <c r="A26" s="9"/>
-      <c r="B26" s="19">
+    <row r="26" spans="1:9" ht="55.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="16">
         <v>22</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="21">
         <v>8</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="21">
         <v>7</v>
       </c>
       <c r="G26" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="27" t="s">
+      <c r="H26" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="27" t="s">
+      <c r="I26" s="32" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="51">
-      <c r="A27" s="9"/>
-      <c r="B27" s="19">
+    <row r="27" spans="1:9" ht="55.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="16">
         <v>23</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E27" s="21">
         <v>8</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="21">
         <v>7</v>
       </c>
       <c r="G27" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="27" t="s">
+      <c r="H27" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="32" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="9"/>
-      <c r="B28" s="19">
+      <c r="A28" s="8"/>
+      <c r="B28" s="16">
         <v>24</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="9"/>
-      <c r="B29" s="19">
+      <c r="A29" s="8"/>
+      <c r="B29" s="16">
         <v>25</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="9"/>
-      <c r="B30" s="18">
+      <c r="A30" s="8"/>
+      <c r="B30" s="15">
         <v>26</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
       <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="9"/>
-      <c r="B31" s="19">
+      <c r="A31" s="8"/>
+      <c r="B31" s="16">
         <v>27</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="9"/>
-      <c r="B32" s="19">
+      <c r="A32" s="8"/>
+      <c r="B32" s="16">
         <v>28</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="9"/>
-      <c r="B33" s="19">
+      <c r="A33" s="8"/>
+      <c r="B33" s="16">
         <v>29</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="9"/>
-      <c r="B34" s="19">
+      <c r="A34" s="8"/>
+      <c r="B34" s="16">
         <v>30</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="9"/>
-      <c r="B35" s="18">
+      <c r="A35" s="8"/>
+      <c r="B35" s="15">
         <v>31</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="9"/>
-      <c r="B36" s="19">
+      <c r="A36" s="8"/>
+      <c r="B36" s="16">
         <v>32</v>
       </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="9"/>
-      <c r="B37" s="19">
+      <c r="A37" s="8"/>
+      <c r="B37" s="16">
         <v>33</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="9"/>
-      <c r="B38" s="19">
+      <c r="A38" s="8"/>
+      <c r="B38" s="16">
         <v>34</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
       <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="9"/>
-      <c r="B39" s="18">
+      <c r="A39" s="8"/>
+      <c r="B39" s="15">
         <v>35</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="9"/>
-      <c r="B40" s="19">
+      <c r="A40" s="8"/>
+      <c r="B40" s="16">
         <v>36</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
       <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="9"/>
-      <c r="B41" s="19">
+      <c r="A41" s="8"/>
+      <c r="B41" s="16">
         <v>37</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
       <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="9"/>
-      <c r="B42" s="19">
+      <c r="A42" s="8"/>
+      <c r="B42" s="16">
         <v>38</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
       <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="9"/>
-      <c r="B43" s="19">
+      <c r="A43" s="8"/>
+      <c r="B43" s="16">
         <v>39</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
       <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="9"/>
-      <c r="B44" s="18">
+      <c r="A44" s="8"/>
+      <c r="B44" s="15">
         <v>40</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
       <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="9"/>
-      <c r="B45" s="20"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:I6 B7:B10 H7:I10 C8:G10 B11:I44">
@@ -1931,7 +1953,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="72" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1941,9 +1963,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34.5" customHeight="1">
@@ -2008,7 +2030,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" thickBot="1">
+    <row r="7" spans="1:8" ht="18" thickBot="1">
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -2204,8 +2226,8 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="14" spans="1:8" ht="18.75" thickBot="1">
+    <row r="13" spans="1:8" ht="13.8" thickBot="1"/>
+    <row r="14" spans="1:8" ht="18" thickBot="1">
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Adds remaining pages to the backlog
</commit_message>
<xml_diff>
--- a/Product Backlog/ProductBacklog-1.xlsx
+++ b/Product Backlog/ProductBacklog-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\repo_my\COSC2299_Group8_Major_Assessment\Product Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rylan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D55E53-9A52-402B-ACA9-EF26EC98DE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86368207-2671-4AAF-9D8E-118B97366612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="3090" windowWidth="16200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -311,6 +311,36 @@
   </si>
   <si>
     <t>Access and edit user information from the database.</t>
+  </si>
+  <si>
+    <t>View medication/symptoms page</t>
+  </si>
+  <si>
+    <t>Given that I am a patient, when I go to view my medication and symptoms, then I have a clear view of the medication that I need to take as well as the ability to edit my symptoms</t>
+  </si>
+  <si>
+    <t>View medication details</t>
+  </si>
+  <si>
+    <t>Given that I am a patient, when I click to see details of a medication, then I can see information such as when I last took the medication, when I can next take it, and the script to get it from the pharmacy if needed</t>
+  </si>
+  <si>
+    <t>Edit symptoms</t>
+  </si>
+  <si>
+    <t>Given that I am a patient, when I want to edit or add a symptom, then there is a clear way to do so linking from the main view symptoms page to this page</t>
+  </si>
+  <si>
+    <t>Accesses and edits user information from the database, will be displayed over the view medication/symptoms page</t>
+  </si>
+  <si>
+    <t>Accesses and edits user information from the database, there will be some variations between patients and doctors for this page such as doctors linking to adding/editing medication as well as being able to edit the doctors notes on the symptoms</t>
+  </si>
+  <si>
+    <t>Add/edit medication</t>
+  </si>
+  <si>
+    <t>Given that I am a doctor, when I need to edit or add a users medication, then I can input the details of the medication as well as the script and it will be added to the list of the patients medication</t>
   </si>
 </sst>
 </file>
@@ -318,10 +348,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1" tint="0.34998626667073579"/>
@@ -520,7 +550,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="5" fontId="5" fillId="0" borderId="3">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0">
@@ -603,13 +633,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -618,13 +648,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -999,26 +1029,26 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" style="22" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" style="22" customWidth="1"/>
-    <col min="8" max="8" width="31.88671875" style="34" customWidth="1"/>
-    <col min="9" max="9" width="62.5546875" style="34" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="22" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="22" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" style="34" customWidth="1"/>
+    <col min="9" max="9" width="62.5703125" style="34" customWidth="1"/>
     <col min="10" max="10" width="2" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="12"/>
+    <col min="11" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" customFormat="1" ht="8.25" customHeight="1">
+    <row r="1" spans="1:9" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1028,7 +1058,7 @@
       <c r="H1" s="29"/>
       <c r="I1" s="29"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="38.25" customHeight="1">
+    <row r="2" spans="1:9" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="8"/>
       <c r="B2" s="14"/>
       <c r="C2" s="18" t="s">
@@ -1041,7 +1071,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="1:9" customFormat="1" ht="6" customHeight="1">
+    <row r="3" spans="1:9" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="8"/>
       <c r="B3" s="14"/>
       <c r="C3" s="19"/>
@@ -1052,7 +1082,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row r="4" spans="1:9" customFormat="1" ht="25.5" customHeight="1">
+    <row r="4" spans="1:9" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>1</v>
@@ -1079,7 +1109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="11" customFormat="1" ht="55.2">
+    <row r="5" spans="1:9" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="15">
         <v>1</v>
@@ -1106,7 +1136,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" ht="55.2">
+    <row r="6" spans="1:9" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="16">
         <v>2</v>
@@ -1133,7 +1163,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="11" customFormat="1" ht="55.2">
+    <row r="7" spans="1:9" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="16">
         <v>3</v>
@@ -1160,7 +1190,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="82.8">
+    <row r="8" spans="1:9" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="16">
         <v>4</v>
@@ -1187,7 +1217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="82.8">
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="16">
         <v>5</v>
@@ -1214,7 +1244,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" ht="110.4">
+    <row r="10" spans="1:9" s="11" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="15">
         <v>6</v>
@@ -1241,7 +1271,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="11" customFormat="1" ht="55.2">
+    <row r="11" spans="1:9" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="16">
         <v>7</v>
@@ -1268,7 +1298,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="11" customFormat="1" ht="69">
+    <row r="12" spans="1:9" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="16">
         <v>8</v>
@@ -1295,7 +1325,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" ht="69">
+    <row r="13" spans="1:9" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="16">
         <v>9</v>
@@ -1322,7 +1352,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" ht="55.2">
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="16">
         <v>10</v>
@@ -1349,7 +1379,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="11" customFormat="1" ht="55.2">
+    <row r="15" spans="1:9" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="15">
         <v>11</v>
@@ -1376,7 +1406,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" ht="55.2">
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="16">
         <v>12</v>
@@ -1403,7 +1433,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" ht="55.2">
+    <row r="17" spans="1:9" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="16">
         <v>13</v>
@@ -1430,7 +1460,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" ht="110.4">
+    <row r="18" spans="1:9" s="11" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="16">
         <v>14</v>
@@ -1457,7 +1487,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" ht="82.8">
+    <row r="19" spans="1:9" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="16">
         <v>15</v>
@@ -1484,7 +1514,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="82.8">
+    <row r="20" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="15">
         <v>16</v>
@@ -1511,7 +1541,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="82.8">
+    <row r="21" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="16">
         <v>17</v>
@@ -1538,7 +1568,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="69">
+    <row r="22" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="16">
         <v>18</v>
@@ -1565,7 +1595,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="69">
+    <row r="23" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="16">
         <v>19</v>
@@ -1592,7 +1622,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="69">
+    <row r="24" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="16">
         <v>20</v>
@@ -1619,7 +1649,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="41.4">
+    <row r="25" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="15">
         <v>21</v>
@@ -1646,7 +1676,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="55.2">
+    <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="16">
         <v>22</v>
@@ -1673,7 +1703,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="55.2">
+    <row r="27" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="16">
         <v>23</v>
@@ -1700,59 +1730,115 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="16">
         <v>24</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="C28" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="21">
+        <v>7</v>
+      </c>
+      <c r="F28" s="21">
+        <v>5</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="16">
         <v>25</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="C29" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="25">
+        <v>5</v>
+      </c>
+      <c r="F29" s="25">
+        <v>4</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="15">
         <v>26</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="C30" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="21">
+        <v>7</v>
+      </c>
+      <c r="F30" s="21">
+        <v>5</v>
+      </c>
+      <c r="G30" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="16">
         <v>27</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="C31" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="21">
+        <v>7</v>
+      </c>
+      <c r="F31" s="21">
+        <v>6</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="16">
         <v>28</v>
@@ -1765,7 +1851,7 @@
       <c r="H32" s="32"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="16">
         <v>29</v>
@@ -1778,7 +1864,7 @@
       <c r="H33" s="32"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="16">
         <v>30</v>
@@ -1791,7 +1877,7 @@
       <c r="H34" s="32"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="15">
         <v>31</v>
@@ -1804,7 +1890,7 @@
       <c r="H35" s="32"/>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="16">
         <v>32</v>
@@ -1817,7 +1903,7 @@
       <c r="H36" s="32"/>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="16">
         <v>33</v>
@@ -1830,7 +1916,7 @@
       <c r="H37" s="32"/>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="16">
         <v>34</v>
@@ -1843,7 +1929,7 @@
       <c r="H38" s="32"/>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="15">
         <v>35</v>
@@ -1856,7 +1942,7 @@
       <c r="H39" s="32"/>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="16">
         <v>36</v>
@@ -1869,7 +1955,7 @@
       <c r="H40" s="32"/>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
       <c r="B41" s="16">
         <v>37</v>
@@ -1882,7 +1968,7 @@
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="16">
         <v>38</v>
@@ -1895,7 +1981,7 @@
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
       <c r="B43" s="16">
         <v>39</v>
@@ -1908,7 +1994,7 @@
       <c r="H43" s="32"/>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="15">
         <v>40</v>
@@ -1921,7 +2007,7 @@
       <c r="H44" s="32"/>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="8"/>
       <c r="B45" s="17"/>
     </row>
@@ -1963,22 +2049,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34.5" customHeight="1">
+    <row r="1" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19.5" customHeight="1">
+    <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -1991,7 +2077,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19.5" customHeight="1">
+    <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -2004,8 +2090,8 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19.5" customHeight="1"/>
-    <row r="6" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2030,7 +2116,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" thickBot="1">
+    <row r="7" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -2056,7 +2142,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="e">
         <f>MATCH(B8,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -2090,7 +2176,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19.5" customHeight="1">
+    <row r="9" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="e">
         <f>MATCH(B9,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -2124,7 +2210,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19.5" customHeight="1">
+    <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="e">
         <f>MATCH(B10,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -2158,7 +2244,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.5" customHeight="1">
+    <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="e">
         <f>MATCH(B11,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -2192,7 +2278,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19.5" customHeight="1">
+    <row r="12" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="e">
         <f>MATCH(B12,'Product Backlog'!$C$5:$C$19,0)</f>
         <v>#REF!</v>
@@ -2226,8 +2312,8 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.8" thickBot="1"/>
-    <row r="14" spans="1:8" ht="18" thickBot="1">
+    <row r="13" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -2238,7 +2324,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="19.5" customHeight="1">
+    <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <f>ROWS($B$15:B15)</f>
         <v>1</v>
@@ -2268,7 +2354,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="19.5" customHeight="1">
+    <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <f>ROWS($B$15:B16)</f>
         <v>2</v>
@@ -2298,7 +2384,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="19.5" customHeight="1">
+    <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <f>ROWS($B$15:B17)</f>
         <v>3</v>
@@ -2328,7 +2414,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="19.5" customHeight="1">
+    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>ROWS($B$15:B18)</f>
         <v>4</v>
@@ -2358,7 +2444,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="19.5" customHeight="1">
+    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>ROWS($B$15:B19)</f>
         <v>5</v>
@@ -2388,7 +2474,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="19.5" customHeight="1">
+    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <f>ROWS($B$15:B20)</f>
         <v>6</v>
@@ -2418,7 +2504,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19.5" customHeight="1">
+    <row r="21" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>ROWS($B$15:B21)</f>
         <v>7</v>
@@ -2448,7 +2534,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="19.5" customHeight="1">
+    <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>ROWS($B$15:B22)</f>
         <v>8</v>
@@ -2478,7 +2564,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="19.5" customHeight="1">
+    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <f>ROWS($B$15:B23)</f>
         <v>9</v>
@@ -2508,7 +2594,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="19.5" customHeight="1">
+    <row r="24" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <f>ROWS($B$15:B24)</f>
         <v>10</v>
@@ -2538,7 +2624,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="19.5" customHeight="1">
+    <row r="25" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>ROWS($B$15:B25)</f>
         <v>11</v>
@@ -2568,7 +2654,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="19.5" customHeight="1">
+    <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>ROWS($B$15:B26)</f>
         <v>12</v>
@@ -2598,7 +2684,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="19.5" customHeight="1">
+    <row r="27" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>ROWS($B$15:B27)</f>
         <v>13</v>
@@ -2628,7 +2714,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="19.5" customHeight="1">
+    <row r="28" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>ROWS($B$15:B28)</f>
         <v>14</v>
@@ -2658,7 +2744,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="19.5" customHeight="1">
+    <row r="29" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>ROWS($B$15:B29)</f>
         <v>15</v>
@@ -2688,7 +2774,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="19.5" customHeight="1">
+    <row r="30" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>ROWS($B$15:B30)</f>
         <v>16</v>
@@ -2718,7 +2804,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="19.5" customHeight="1">
+    <row r="31" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>ROWS($B$15:B31)</f>
         <v>17</v>
@@ -2748,7 +2834,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="19.5" customHeight="1">
+    <row r="32" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <f>ROWS($B$15:B32)</f>
         <v>18</v>
@@ -2778,7 +2864,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="19.5" customHeight="1">
+    <row r="33" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <f>ROWS($B$15:B33)</f>
         <v>19</v>
@@ -2808,7 +2894,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="19.5" customHeight="1">
+    <row r="34" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <f>ROWS($B$15:B34)</f>
         <v>20</v>
@@ -2838,7 +2924,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="19.5" customHeight="1">
+    <row r="35" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <f>ROWS($B$15:B35)</f>
         <v>21</v>
@@ -2868,7 +2954,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="19.5" customHeight="1">
+    <row r="36" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <f>ROWS($B$15:B36)</f>
         <v>22</v>
@@ -2898,7 +2984,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="19.5" customHeight="1">
+    <row r="37" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <f>ROWS($B$15:B37)</f>
         <v>23</v>
@@ -2928,63 +3014,63 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="19.5" customHeight="1">
+    <row r="38" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <f>ROWS($B$15:B38)</f>
         <v>24</v>
       </c>
       <c r="B38" t="str">
         <f>IF('Product Backlog'!C28=0,"",'Product Backlog'!C28)</f>
-        <v/>
+        <v>View medication/symptoms page</v>
       </c>
       <c r="C38" t="e">
-        <f>IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,C$6),NA()))</f>
+        <f ca="1">IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D38" t="e">
-        <f>IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,D$6),NA()))</f>
+        <f ca="1">IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E38" t="e">
-        <f>IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,E$6),NA()))</f>
+        <f ca="1">IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F38" t="e">
-        <f>IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,F$6),NA()))</f>
+        <f ca="1">IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G38" t="e">
-        <f>IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,G$6),NA()))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="19.5" customHeight="1">
+        <f ca="1">IF(B38="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A38,G$6),NA()))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <f>ROWS($B$15:B39)</f>
         <v>25</v>
       </c>
       <c r="B39" t="str">
         <f>IF('Product Backlog'!C29=0,"",'Product Backlog'!C29)</f>
-        <v/>
+        <v>View medication details</v>
       </c>
       <c r="C39" t="e">
-        <f>IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,C$6),NA()))</f>
+        <f ca="1">IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,C$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="D39" t="e">
-        <f>IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,D$6),NA()))</f>
+        <f ca="1">IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,D$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="E39" t="e">
-        <f>IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,E$6),NA()))</f>
+        <f ca="1">IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,E$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="F39" t="e">
-        <f>IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,F$6),NA()))</f>
+        <f ca="1">IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,F$6),NA()))</f>
         <v>#N/A</v>
       </c>
       <c r="G39" t="e">
-        <f>IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,G$6),NA()))</f>
+        <f ca="1">IF(B39="",NA(),IFERROR(INDEX('Product Backlog'!$C$5:$I$29,$A39,G$6),NA()))</f>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>